<commit_message>
Adding screening visit logic
</commit_message>
<xml_diff>
--- a/simplifiedPreventiveServices.xlsx
+++ b/simplifiedPreventiveServices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burke/Documents/research/scrooge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53220AB5-4F53-0549-BCF9-5F3595EF9EC9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C9CCB6-8ACF-8949-BE96-BDCD3CA55A58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="8460" windowWidth="35320" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
+    <workbookView xWindow="0" yWindow="2960" windowWidth="33600" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,12 +149,6 @@
     <t>Hep A and Hep B</t>
   </si>
   <si>
-    <t>Min Age</t>
-  </si>
-  <si>
-    <t>Max Age</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>Smoking</t>
   </si>
   <si>
-    <t>Current, Former</t>
-  </si>
-  <si>
     <t>Never</t>
   </si>
   <si>
@@ -243,12 +234,24 @@
   </si>
   <si>
     <t>q15</t>
+  </si>
+  <si>
+    <t>minAge</t>
+  </si>
+  <si>
+    <t>maxAge</t>
+  </si>
+  <si>
+    <t>Former</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -347,9 +350,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -365,13 +365,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,7 +694,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+      <selection activeCell="K5" sqref="K5:K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,28 +717,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -746,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2">
         <v>65</v>
@@ -755,10 +758,10 @@
         <v>75</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -772,7 +775,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>65</v>
@@ -781,10 +784,10 @@
         <v>75</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -799,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="2">
         <v>3</v>
@@ -816,12 +819,12 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="13">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
@@ -833,7 +836,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
@@ -848,7 +851,7 @@
       <c r="J6" s="2">
         <v>2.5</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="13">
         <v>0.2</v>
       </c>
     </row>
@@ -860,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
@@ -875,19 +878,19 @@
       <c r="J7" s="2">
         <v>2.5</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="13">
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2">
         <v>18</v>
@@ -898,19 +901,19 @@
       <c r="J8" s="2">
         <v>1.5</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="13">
         <v>0.7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2">
         <v>25</v>
@@ -918,19 +921,19 @@
       <c r="J9" s="2">
         <v>1.5</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="13">
         <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2">
         <v>18</v>
@@ -939,26 +942,27 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J10" s="2">
         <v>3</v>
       </c>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J11" s="2">
         <v>3</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="13">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
@@ -979,64 +983,66 @@
         <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
       </c>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2">
         <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2">
         <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="13">
         <v>0.24</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2">
         <v>18</v>
@@ -1047,7 +1053,7 @@
       <c r="J15" s="2">
         <v>1</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="13">
         <v>0.24</v>
       </c>
     </row>
@@ -1059,24 +1065,24 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="13">
         <v>0.34</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>57</v>
+      <c r="A17" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2">
         <v>55</v>
@@ -1087,19 +1093,19 @@
       <c r="J17" s="2">
         <v>1</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="13">
         <v>0.17</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>58</v>
+      <c r="A18" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2">
         <v>65</v>
@@ -1110,19 +1116,19 @@
       <c r="J18" s="2">
         <v>1</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="13">
         <v>0.125</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>59</v>
+      <c r="A19" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2">
         <v>75</v>
@@ -1133,59 +1139,59 @@
       <c r="J19" s="2">
         <v>1</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="13">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>60</v>
+      <c r="A20" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="6">
         <v>18</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>64</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="2">
         <v>1</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="14">
         <v>0.1411</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>61</v>
+      <c r="A21" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="6">
         <v>65</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="2">
         <v>1</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="14">
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
@@ -1197,55 +1203,56 @@
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
       </c>
+      <c r="K22" s="13"/>
     </row>
     <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
       <c r="J23" s="2">
         <v>1</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="13">
         <v>0.97099999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
       <c r="J24" s="2">
         <v>1</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="13">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
@@ -1257,11 +1264,12 @@
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J25" s="2">
         <v>0.25</v>
       </c>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -1271,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D26" s="2">
         <v>53</v>
@@ -1282,7 +1290,7 @@
       <c r="J26" s="2">
         <v>1</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -1300,7 +1308,7 @@
       <c r="J27" s="2">
         <v>1</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="13">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
@@ -1323,30 +1331,30 @@
       <c r="J28" s="2">
         <v>1</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="13">
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="C29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="2">
         <v>1</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="13">
         <v>8.1000000000000003E-2</v>
       </c>
     </row>
@@ -1358,7 +1366,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
@@ -1366,6 +1374,7 @@
       <c r="J30" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="K30" s="13"/>
     </row>
     <row r="31" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -1375,7 +1384,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H31" s="2">
         <v>1</v>
@@ -1383,6 +1392,7 @@
       <c r="J31" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -1392,14 +1402,15 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D32" s="2">
         <v>65</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="11">
         <v>0.75</v>
       </c>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1409,34 +1420,36 @@
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D33" s="2">
         <v>65</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="12">
         <v>0.75</v>
       </c>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="C34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="2">
         <v>0.5</v>
       </c>
+      <c r="K34" s="13"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
@@ -1446,11 +1459,12 @@
         <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
       </c>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
@@ -1460,21 +1474,22 @@
         <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
       </c>
+      <c r="K36" s="13"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -1485,19 +1500,19 @@
       <c r="J37" s="2">
         <v>1</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="13">
         <v>0.24</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2">
         <v>21</v>
@@ -1508,9 +1523,10 @@
       <c r="J38" s="2">
         <v>1</v>
       </c>
+      <c r="K38" s="13"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1528,9 +1544,10 @@
       <c r="J39" s="2">
         <v>1</v>
       </c>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1548,6 +1565,7 @@
       <c r="J40" s="2">
         <v>1</v>
       </c>
+      <c r="K40" s="13"/>
     </row>
     <row r="41" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -1557,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D41" s="2">
         <v>35</v>
@@ -1568,19 +1586,19 @@
       <c r="J41" s="2">
         <v>1.5</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="13">
         <v>0.155</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1591,19 +1609,19 @@
       <c r="J42" s="2">
         <v>1</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="13">
         <v>0.11</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" s="2">
         <v>50</v>
@@ -1614,19 +1632,19 @@
       <c r="J43" s="2">
         <v>1.5</v>
       </c>
-      <c r="K43" s="6">
+      <c r="K43" s="13">
         <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D44" s="2">
         <v>50</v>
@@ -1637,36 +1655,36 @@
       <c r="J44" s="2">
         <v>1.5</v>
       </c>
-      <c r="K44" s="6">
+      <c r="K44" s="13">
         <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J45" s="2">
         <v>5</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="13">
         <v>0.3</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D46" s="2">
         <v>40</v>
@@ -1680,84 +1698,91 @@
       <c r="J46" s="2">
         <v>12.2</v>
       </c>
+      <c r="K46" s="13"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J47" s="2">
         <v>0.5</v>
       </c>
+      <c r="K47" s="13"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J48" s="2">
         <v>0.5</v>
       </c>
+      <c r="K48" s="13"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J49" s="2">
         <v>0.5</v>
       </c>
+      <c r="K49" s="13"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J50" s="2">
         <v>0.5</v>
       </c>
+      <c r="K50" s="13"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J51" s="2">
         <v>0.5</v>
       </c>
+      <c r="K51" s="13"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J52" s="2">
         <v>0.5</v>
       </c>
+      <c r="K52" s="13"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J53" s="2">
         <v>0.5</v>
       </c>
-      <c r="K53" s="6">
+      <c r="K53" s="13">
         <v>0.13950000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding tests and fixing screening logic
</commit_message>
<xml_diff>
--- a/simplifiedPreventiveServices.xlsx
+++ b/simplifiedPreventiveServices.xlsx
@@ -8,22 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burke/Documents/research/scrooge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C9CCB6-8ACF-8949-BE96-BDCD3CA55A58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A00683F-56F4-F34D-95DC-DB7D5D4B7906}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2960" windowWidth="33600" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
+    <workbookView xWindow="200" yWindow="440" windowWidth="33600" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -694,7 +690,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K53"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +848,7 @@
         <v>2.5</v>
       </c>
       <c r="K6" s="13">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
screening logic performance and fixing/testing visits
</commit_message>
<xml_diff>
--- a/simplifiedPreventiveServices.xlsx
+++ b/simplifiedPreventiveServices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burke/Documents/research/scrooge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A00683F-56F4-F34D-95DC-DB7D5D4B7906}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7B6E6-345E-6344-847F-A296107DBC6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="440" windowWidth="33600" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>Service</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Healthful Diet and Physical Activity for Cardiovascular Disease Prevention in Adults Without Known Risk Factors: Behavioral Counseling</t>
   </si>
   <si>
-    <t>12.2 min</t>
-  </si>
-  <si>
     <t>Healthful Diet and Physical Activity for Cardiovascular Disease Prevention in Adults With Cardiovascular Risk Factors: Behavioral Counseling</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Never</t>
   </si>
   <si>
-    <t>Once</t>
-  </si>
-  <si>
     <t>Current</t>
   </si>
   <si>
@@ -239,6 +233,9 @@
   </si>
   <si>
     <t>Former</t>
+  </si>
+  <si>
+    <t>q-1</t>
   </si>
 </sst>
 </file>
@@ -690,7 +687,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,28 +710,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -745,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2">
         <v>65</v>
@@ -754,10 +751,10 @@
         <v>75</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
@@ -771,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2">
         <v>65</v>
@@ -780,10 +777,10 @@
         <v>75</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -798,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2">
         <v>3</v>
@@ -815,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -832,7 +829,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="5">
         <v>40</v>
@@ -859,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="5">
         <v>40</v>
@@ -886,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2">
         <v>18</v>
@@ -897,9 +894,7 @@
       <c r="J8" s="2">
         <v>1.5</v>
       </c>
-      <c r="K8" s="13">
-        <v>0.7</v>
-      </c>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -909,7 +904,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2">
         <v>25</v>
@@ -923,13 +918,13 @@
     </row>
     <row r="10" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>18</v>
@@ -938,7 +933,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J10" s="2">
         <v>3</v>
@@ -947,13 +942,13 @@
     </row>
     <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J11" s="2">
         <v>3</v>
@@ -970,7 +965,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>55</v>
@@ -979,7 +974,7 @@
         <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -988,19 +983,19 @@
     </row>
     <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2">
         <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1009,19 +1004,19 @@
     </row>
     <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2">
         <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1032,13 +1027,13 @@
     </row>
     <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2">
         <v>18</v>
@@ -1061,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
@@ -1072,13 +1067,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2">
         <v>55</v>
@@ -1095,13 +1090,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2">
         <v>65</v>
@@ -1118,13 +1113,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2">
         <v>75</v>
@@ -1141,13 +1136,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>43</v>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D20" s="6">
         <v>18</v>
@@ -1168,13 +1163,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>43</v>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D21" s="6">
         <v>65</v>
@@ -1199,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -1208,13 +1203,13 @@
     </row>
     <row r="23" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>43</v>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1231,13 +1226,13 @@
     </row>
     <row r="24" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1260,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J25" s="2">
         <v>0.25</v>
@@ -1275,7 +1270,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2">
         <v>53</v>
@@ -1296,7 +1291,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2">
         <v>74</v>
@@ -1316,7 +1311,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="2">
         <v>18</v>
@@ -1339,7 +1334,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1362,43 +1357,43 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>19</v>
+      <c r="J30" s="2">
+        <v>12.2</v>
       </c>
       <c r="K30" s="13"/>
     </row>
     <row r="31" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H31" s="2">
         <v>1</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>19</v>
+      <c r="J31" s="2">
+        <v>12.2</v>
       </c>
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D32" s="2">
         <v>65</v>
@@ -1410,13 +1405,13 @@
     </row>
     <row r="33" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2">
         <v>65</v>
@@ -1428,13 +1423,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1449,13 +1444,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J35" s="2">
         <v>1</v>
@@ -1464,13 +1459,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J36" s="2">
         <v>1</v>
@@ -1479,13 +1474,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -1502,13 +1497,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D38" s="2">
         <v>21</v>
@@ -1523,13 +1518,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D39" s="2">
         <v>50</v>
@@ -1544,13 +1539,13 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" s="2">
         <v>40</v>
@@ -1565,13 +1560,13 @@
     </row>
     <row r="41" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D41" s="2">
         <v>35</v>
@@ -1588,13 +1583,13 @@
     </row>
     <row r="42" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1611,13 +1606,13 @@
     </row>
     <row r="43" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D43" s="2">
         <v>50</v>
@@ -1634,13 +1629,13 @@
     </row>
     <row r="44" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D44" s="2">
         <v>50</v>
@@ -1657,13 +1652,13 @@
     </row>
     <row r="45" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J45" s="2">
         <v>5</v>
@@ -1674,13 +1669,13 @@
     </row>
     <row r="46" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2">
         <v>40</v>
@@ -1698,10 +1693,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J47" s="2">
         <v>0.5</v>
@@ -1710,10 +1705,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J48" s="2">
         <v>0.5</v>
@@ -1722,10 +1717,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J49" s="2">
         <v>0.5</v>
@@ -1734,10 +1729,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J50" s="2">
         <v>0.5</v>
@@ -1746,10 +1741,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J51" s="2">
         <v>0.5</v>
@@ -1758,10 +1753,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J52" s="2">
         <v>0.5</v>
@@ -1770,10 +1765,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J53" s="2">
         <v>0.5</v>

</xml_diff>

<commit_message>
Adding additional provider variables
</commit_message>
<xml_diff>
--- a/simplifiedPreventiveServices.xlsx
+++ b/simplifiedPreventiveServices.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burke/Documents/research/scrooge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE7B6E6-345E-6344-847F-A296107DBC6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59795BB-25DA-9540-B5E8-7F22D2B7366B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="440" windowWidth="33600" windowHeight="16940" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
+    <workbookView xWindow="200" yWindow="440" windowWidth="37020" windowHeight="22440" xr2:uid="{4552D074-C7DE-9A49-AD44-EC0C43D3616C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="70">
   <si>
     <t>Service</t>
   </si>
@@ -686,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E61C7B-7791-7A4B-9D53-E941958244DB}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,7 +980,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
@@ -1002,7 +1001,7 @@
       </c>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -1367,7 +1366,7 @@
       </c>
       <c r="K30" s="13"/>
     </row>
-    <row r="31" spans="1:11" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>19</v>
       </c>
@@ -1385,7 +1384,7 @@
       </c>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1402,7 @@
       </c>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>20</v>
       </c>
@@ -1421,7 +1420,7 @@
       </c>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
@@ -1442,7 +1441,7 @@
       </c>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
@@ -1457,7 +1456,7 @@
       </c>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
@@ -1472,7 +1471,7 @@
       </c>
       <c r="K36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>23</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>24</v>
       </c>
@@ -1511,12 +1510,15 @@
       <c r="E38" s="2">
         <v>65</v>
       </c>
+      <c r="F38" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J38" s="2">
         <v>1</v>
       </c>
       <c r="K38" s="13"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>25</v>
       </c>
@@ -1532,12 +1534,15 @@
       <c r="E39" s="2">
         <v>74</v>
       </c>
+      <c r="F39" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J39" s="2">
         <v>1</v>
       </c>
       <c r="K39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>25</v>
       </c>
@@ -1553,12 +1558,15 @@
       <c r="E40" s="2">
         <v>50</v>
       </c>
+      <c r="F40" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J40" s="2">
         <v>1</v>
       </c>
       <c r="K40" s="13"/>
     </row>
-    <row r="41" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>27</v>
       </c>
@@ -1574,6 +1582,9 @@
       <c r="E41" s="2">
         <v>79</v>
       </c>
+      <c r="F41" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J41" s="2">
         <v>1.5</v>
       </c>
@@ -1581,7 +1592,7 @@
         <v>0.155</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>28</v>
       </c>
@@ -1593,7 +1604,9 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -1604,7 +1617,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>29</v>
       </c>
@@ -1627,7 +1640,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>29</v>
       </c>
@@ -1650,7 +1663,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
@@ -1667,7 +1680,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>31</v>
       </c>
@@ -1691,7 +1704,7 @@
       </c>
       <c r="K46" s="13"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>32</v>
       </c>
@@ -1703,7 +1716,7 @@
       </c>
       <c r="K47" s="13"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>33</v>
       </c>
@@ -1715,7 +1728,7 @@
       </c>
       <c r="K48" s="13"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
@@ -1727,7 +1740,7 @@
       </c>
       <c r="K49" s="13"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>35</v>
       </c>
@@ -1739,7 +1752,7 @@
       </c>
       <c r="K50" s="13"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>36</v>
       </c>
@@ -1751,7 +1764,7 @@
       </c>
       <c r="K51" s="13"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>36</v>
       </c>
@@ -1763,7 +1776,7 @@
       </c>
       <c r="K52" s="13"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>

</xml_diff>